<commit_message>
added new active space
</commit_message>
<xml_diff>
--- a/bimetallics/fe2s2_sharma/32__3d4d_2p3p/tpsci_01.xlsx
+++ b/bimetallics/fe2s2_sharma/32__3d4d_2p3p/tpsci_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nmayhall/code/FermiCG-data/bimetallics/fe2s2_sharma/32__3d4d_2p3p/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A773672E-E33A-F24D-959C-A124ADE835F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CEB2ABD-AB69-BC4C-AD0B-DBE8A6C8668C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="3" xr2:uid="{47E1590A-DBCB-6240-B749-9F1759EEA5AE}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{47E1590A-DBCB-6240-B749-9F1759EEA5AE}"/>
   </bookViews>
   <sheets>
     <sheet name="m050" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -60,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="23">
   <si>
     <t>E0i:</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Delta PT2</t>
+  </si>
+  <si>
+    <t>BST</t>
   </si>
 </sst>
 </file>
@@ -3195,644 +3198,6 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:lineChart>
-        <c:grouping val="standard"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'m100'!$L$20</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Extrapolated</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'m100'!$L$21:$L$26</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>111.93881518663467</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>319.19712771672846</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>611.18128780292875</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1011.6554661708877</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1522.8647558032471</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-147B-2E46-AF0C-5F8031D49638}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'m100'!$M$20</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Variational</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'m100'!$M$21:$M$26</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>95.014956818370209</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>285.3784718953616</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>572.38983503891552</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>958.06601809875474</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1444.5359249873659</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-147B-2E46-AF0C-5F8031D49638}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="2"/>
-          <c:order val="2"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'m100'!$N$20</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>PT2</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'m100'!$N$21:$N$26</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>97.714494769287512</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>295.52917353218487</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>594.25609242762243</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>994.50319617018272</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1497.8902075385254</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000002-147B-2E46-AF0C-5F8031D49638}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="3"/>
-          <c:order val="3"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'m100'!$O$20</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Heisenberg</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'m100'!$O$21:$O$26</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="6"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>111.93881518663467</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>335.81644555990403</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>671.63289111980805</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1119.3881518663468</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1679.0822277995203</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-147B-2E46-AF0C-5F8031D49638}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:marker val="1"/>
-        <c:smooth val="0"/>
-        <c:axId val="1277389312"/>
-        <c:axId val="2048151680"/>
-      </c:lineChart>
-      <c:catAx>
-        <c:axId val="1277389312"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Spin,</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> S</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2048151680"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2048151680"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="2000"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Energy Gap, cm-1</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="1277389312"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="tr"/>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.18934667541557307"/>
-          <c:y val="6.4122145112958481E-2"/>
-          <c:w val="0.21229704054652934"/>
-          <c:h val="0.30635618978119411"/>
-        </c:manualLayout>
-      </c:layout>
-      <c:overlay val="1"/>
-      <c:spPr>
-        <a:solidFill>
-          <a:schemeClr val="bg1"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:extLst>
-      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
-        <c16r3:dataDisplayOptions16>
-          <c16r3:dispNaAsBlank val="1"/>
-        </c16r3:dataDisplayOptions16>
-      </c:ext>
-    </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
     <c:title>
       <c:tx>
         <c:rich>
@@ -6081,6 +5446,716 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'m100'!$L$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Extrapolated</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'m100'!$L$21:$L$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>111.93881518663467</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>319.19712771672846</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>611.18128780292875</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1011.6554661708877</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1522.8647558032471</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1996-C54F-B8A7-919F1D2A2609}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'m100'!$M$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Variational</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'m100'!$M$21:$M$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>95.014956818370209</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>285.3784718953616</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>572.38983503891552</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>958.06601809875474</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1444.5359249873659</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1996-C54F-B8A7-919F1D2A2609}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'m100'!$N$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>PT2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'m100'!$N$21:$N$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>97.714494769287512</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>295.52917353218487</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>594.25609242762243</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>994.50319617018272</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1497.8902075385254</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1996-C54F-B8A7-919F1D2A2609}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'m100'!$O$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Heisenberg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'m100'!$O$21:$O$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>111.93881518663467</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>335.81644555990403</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>671.63289111980805</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1119.3881518663468</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1679.0822277995203</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-1996-C54F-B8A7-919F1D2A2609}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'m100'!$P$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>BST</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'m100'!$P$21:$P$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>83.556186387679077</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>289.52215290952984</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>585.54294961616472</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>979.59867405032958</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1467.0254903238238</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-1996-C54F-B8A7-919F1D2A2609}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1277389312"/>
+        <c:axId val="2048151680"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1277389312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Spin,</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0"/>
+                  <a:t> S</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2048151680"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2048151680"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2000"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Energy Gap, cm-1</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1277389312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="tr"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18934667541557307"/>
+          <c:y val="6.4122145112958481E-2"/>
+          <c:w val="0.21378455762710044"/>
+          <c:h val="0.3848166270144095"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -12142,7 +12217,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -12169,8 +12244,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -12271,7 +12346,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -12303,10 +12378,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -12346,22 +12421,23 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -12466,8 +12542,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -12599,19 +12675,20 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525">
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
+        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -12625,6 +12702,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -12645,7 +12733,7 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="332">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -12672,8 +12760,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -12774,7 +12862,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -12806,10 +12894,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -12849,23 +12937,22 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
         </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:downBar>
@@ -12970,8 +13057,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -13103,20 +13190,19 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
         <a:schemeClr val="lt1"/>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
-        <a:round/>
       </a:ln>
     </cs:spPr>
   </cs:upBar>
@@ -13130,17 +13216,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -15298,21 +15373,21 @@
     <xdr:from>
       <xdr:col>16</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>444500</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>131233</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>561340</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="8" name="Chart 7">
+        <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6F726607-AA70-0C4D-8F39-1EC633DB020D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BD626FC-7E13-B843-BD91-8E496C2F0ED7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -15334,23 +15409,23 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>561340</xdr:colOff>
-      <xdr:row>53</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>131233</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
+        <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BD626FC-7E13-B843-BD91-8E496C2F0ED7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{019DFDD7-C564-2B46-8DFC-188D69CA0286}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -17073,10 +17148,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AC8F4FA-95EA-5649-B8CB-32F8EE08E78A}">
-  <dimension ref="A1:P63"/>
+  <dimension ref="A1:Q63"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="168" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17556,7 +17631,7 @@
         <v>-78.026839789999997</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C17">
         <v>5</v>
       </c>
@@ -17589,7 +17664,7 @@
         <v>-78.025002909999998</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C18">
         <v>6</v>
       </c>
@@ -17622,7 +17697,7 @@
         <v>-78.022749230000002</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.2">
       <c r="L19" s="9" t="s">
         <v>20</v>
       </c>
@@ -17630,12 +17705,15 @@
       <c r="N19" s="9"/>
       <c r="O19" s="9"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.2">
       <c r="I20" s="1" t="s">
         <v>3</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="K20" t="s">
+        <v>22</v>
       </c>
       <c r="L20" s="1" t="str">
         <f>J20</f>
@@ -17650,11 +17728,15 @@
       <c r="O20" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="P20" s="1" t="s">
+      <c r="P20" t="str">
+        <f>K20</f>
+        <v>BST</v>
+      </c>
+      <c r="Q20" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C21">
         <f>C13</f>
         <v>1</v>
@@ -17678,6 +17760,9 @@
       <c r="J21" s="1">
         <v>-78.030078080160607</v>
       </c>
+      <c r="K21">
+        <v>-78.030294019999999</v>
+      </c>
       <c r="L21" s="3">
         <f>$A$1*(J21-J$21)</f>
         <v>0</v>
@@ -17693,12 +17778,16 @@
       <c r="O21" s="3">
         <v>0</v>
       </c>
-      <c r="P21" s="2">
+      <c r="P21" s="3">
+        <f>$A$1*(K21-K$21)</f>
+        <v>0</v>
+      </c>
+      <c r="Q21" s="2">
         <f>(J21-J22)*$A$1/C21/2</f>
         <v>-55.969407593317335</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C22">
         <f t="shared" ref="C22:C26" si="4">C14</f>
         <v>2</v>
@@ -17722,6 +17811,9 @@
       <c r="J22" s="1">
         <v>-78.029568049387635</v>
       </c>
+      <c r="K22">
+        <v>-78.029913309999998</v>
+      </c>
       <c r="L22" s="3">
         <f t="shared" ref="L22:L26" si="5">$A$1*(J22-J$21)</f>
         <v>111.93881518663467</v>
@@ -17735,15 +17827,19 @@
         <v>97.714494769287512</v>
       </c>
       <c r="O22" s="3">
-        <f>O21-2*P$21*C21</f>
+        <f>O21-2*Q$21*C21</f>
         <v>111.93881518663467</v>
       </c>
-      <c r="P22" s="2">
+      <c r="P22" s="3">
+        <f t="shared" ref="P22:P26" si="8">$A$1*(K22-K$21)</f>
+        <v>83.556186387679077</v>
+      </c>
+      <c r="Q22" s="2">
         <f>(J22-J23)*$A$1/C22/2</f>
         <v>-51.814578132523444</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C23">
         <f t="shared" si="4"/>
         <v>3</v>
@@ -17767,6 +17863,9 @@
       <c r="J23" s="1">
         <v>-78.028623711025929</v>
       </c>
+      <c r="K23">
+        <v>-78.028974860000005</v>
+      </c>
       <c r="L23" s="3">
         <f t="shared" si="5"/>
         <v>319.19712771672846</v>
@@ -17780,15 +17879,19 @@
         <v>295.52917353218487</v>
       </c>
       <c r="O23" s="3">
-        <f t="shared" ref="O23:O26" si="8">O22-2*P$21*C22</f>
+        <f>O22-2*Q$21*C22</f>
         <v>335.81644555990403</v>
       </c>
-      <c r="P23" s="2">
+      <c r="P23" s="3">
+        <f t="shared" si="8"/>
+        <v>289.52215290952984</v>
+      </c>
+      <c r="Q23" s="2">
         <f>(J23-J24)*$A$1/C23/2</f>
         <v>-48.664026681033384</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="C24">
         <f t="shared" si="4"/>
@@ -17813,6 +17916,9 @@
       <c r="J24" s="1">
         <v>-78.027293333295773</v>
       </c>
+      <c r="K24">
+        <v>-78.027626089999998</v>
+      </c>
       <c r="L24" s="3">
         <f t="shared" si="5"/>
         <v>611.18128780292875</v>
@@ -17826,15 +17932,19 @@
         <v>594.25609242762243</v>
       </c>
       <c r="O24" s="3">
+        <f>O23-2*Q$21*C23</f>
+        <v>671.63289111980805</v>
+      </c>
+      <c r="P24" s="3">
         <f t="shared" si="8"/>
-        <v>671.63289111980805</v>
-      </c>
-      <c r="P24" s="2">
+        <v>585.54294961616472</v>
+      </c>
+      <c r="Q24" s="2">
         <f>(J24-J25)*$A$1/C24/2</f>
         <v>-50.05927229599488</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C25">
         <f t="shared" si="4"/>
         <v>5</v>
@@ -17858,6 +17968,9 @@
       <c r="J25" s="1">
         <v>-78.025468638667661</v>
       </c>
+      <c r="K25">
+        <v>-78.025830639999995</v>
+      </c>
       <c r="L25" s="3">
         <f t="shared" si="5"/>
         <v>1011.6554661708877</v>
@@ -17871,15 +17984,19 @@
         <v>994.50319617018272</v>
       </c>
       <c r="O25" s="3">
+        <f>O24-2*Q$21*C24</f>
+        <v>1119.3881518663468</v>
+      </c>
+      <c r="P25" s="3">
         <f t="shared" si="8"/>
-        <v>1119.3881518663468</v>
-      </c>
-      <c r="P25" s="2">
+        <v>979.59867405032958</v>
+      </c>
+      <c r="Q25" s="2">
         <f>(J25-J26)*$A$1/C25/2</f>
         <v>-51.120928963235947</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C26">
         <f t="shared" si="4"/>
         <v>6</v>
@@ -17903,6 +18020,9 @@
       <c r="J26" s="1">
         <v>-78.023139397745226</v>
       </c>
+      <c r="K26">
+        <v>-78.023609759999999</v>
+      </c>
       <c r="L26" s="3">
         <f t="shared" si="5"/>
         <v>1522.8647558032471</v>
@@ -17916,8 +18036,12 @@
         <v>1497.8902075385254</v>
       </c>
       <c r="O26" s="3">
+        <f>O25-2*Q$21*C25</f>
+        <v>1679.0822277995203</v>
+      </c>
+      <c r="P26" s="3">
         <f t="shared" si="8"/>
-        <v>1679.0822277995203</v>
+        <v>1467.0254903238238</v>
       </c>
     </row>
     <row r="34" spans="4:16" x14ac:dyDescent="0.2">
@@ -19580,7 +19704,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{623568B5-478C-6A41-BC81-0B52F21DD4B5}">
   <dimension ref="B1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
@@ -19715,25 +19839,25 @@
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17">
-        <f>B2</f>
+        <f t="shared" ref="B17:B22" si="0">B2</f>
         <v>1</v>
       </c>
       <c r="C17">
-        <f t="shared" ref="C17:E17" si="0">(C2-C$2)*1000</f>
+        <f t="shared" ref="C17:E17" si="1">(C2-C$2)*1000</f>
         <v>0</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="E17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18">
-        <f>B3</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="C18">
@@ -19741,83 +19865,83 @@
         <v>0.48755876777306639</v>
       </c>
       <c r="D18">
-        <f t="shared" ref="D18:E18" si="1">(D3-D$2)*1000</f>
+        <f t="shared" ref="D18:E18" si="2">(D3-D$2)*1000</f>
         <v>0.51003077297195887</v>
       </c>
       <c r="E18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.57685161637266447</v>
       </c>
     </row>
     <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19">
-        <f>B4</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="C19">
-        <f t="shared" ref="C19:E19" si="2">(C4-C$2)*1000</f>
+        <f t="shared" ref="C19:E19" si="3">(C4-C$2)*1000</f>
         <v>1.3902180819798104</v>
       </c>
       <c r="D19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.4543691346773358</v>
       </c>
       <c r="E19">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.5849219908403711</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20">
-        <f>B5</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="C20">
-        <f t="shared" ref="C20:E20" si="3">(C5-C$2)*1000</f>
+        <f t="shared" ref="C20:E20" si="4">(C5-C$2)*1000</f>
         <v>2.6958289163729887</v>
       </c>
       <c r="D20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.7847468648332097</v>
       </c>
       <c r="E20">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.8361929829401333</v>
       </c>
     </row>
     <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21">
-        <f>B6</f>
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="C21">
-        <f t="shared" ref="C21:E21" si="4">(C6-C$2)*1000</f>
+        <f t="shared" ref="C21:E21" si="5">(C6-C$2)*1000</f>
         <v>4.4788284706243076</v>
       </c>
       <c r="D21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.6094414929456207</v>
       </c>
       <c r="E21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.5971423584774129</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22">
-        <f>B7</f>
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="C22">
-        <f t="shared" ref="C22:E22" si="5">(C7-C$2)*1000</f>
+        <f t="shared" ref="C22:E22" si="6">(C7-C$2)*1000</f>
         <v>6.7473199266601114</v>
       </c>
       <c r="D22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.9386824153809812</v>
       </c>
       <c r="E22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.881298085673393</v>
       </c>
     </row>

</xml_diff>